<commit_message>
Adicionando automação do jadlog e correção do Integratedlogger
</commit_message>
<xml_diff>
--- a/ProjetoFinalCompass/Processar/Planilha de Entrada Grupos.xlsx
+++ b/ProjetoFinalCompass/Processar/Planilha de Entrada Grupos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projeto_Final_Compass\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RPA\ProjetoFinalCompass\Processar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6105FB-78C1-492A-B5D0-81F3EE79541D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4814FCA-55C8-4082-B388-BE78215DDC06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -523,7 +523,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>